<commit_message>
Fix efficirentnet-b0 accuracy checker results
</commit_message>
<xml_diff>
--- a/results/accuracy/TVM-0.14-public_models-2023-12-20.xlsx
+++ b/results/accuracy/TVM-0.14-public_models-2023-12-20.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Task type</t>
   </si>
@@ -40,9 +40,6 @@
     <t>TVM</t>
   </si>
   <si>
-    <t>CPU: Intel(R) Xeon(R) Gold 6138 CPU @ 2.00GHz, CPU family: x86_64, GPU: Undefined, RAM size: 526950192 kB, OS family: Linux, OS version: Linux-5.15.0-84-generic-x86_64-with-glibc2.29, Python version: 3.8.10</t>
-  </si>
-  <si>
     <t>CPU: Intel(R) Core(TM) i7-8700 CPU @ 3.20GHz, CPU family: x86_64, GPU: Undefined, RAM size: 65702408 kB, OS family: Linux, OS version: Linux-5.15.0-84-generic-x86_64-with-glibc2.29, Python version: 3.8.10</t>
   </si>
   <si>
@@ -61,64 +58,64 @@
     <t>accuracy@top1</t>
   </si>
   <si>
-    <t>60.88%</t>
+    <t>74.40%</t>
   </si>
   <si>
     <t>accuracy@top5</t>
   </si>
   <si>
-    <t>84.42%</t>
+    <t>92.14%</t>
+  </si>
+  <si>
+    <t>googlenet-v1</t>
+  </si>
+  <si>
+    <t>Caffe</t>
+  </si>
+  <si>
+    <t>68.92%</t>
+  </si>
+  <si>
+    <t>89.14%</t>
+  </si>
+  <si>
+    <t>googlenet-v4-tf</t>
+  </si>
+  <si>
+    <t>80.21%</t>
+  </si>
+  <si>
+    <t>95.19%</t>
+  </si>
+  <si>
+    <t>resnet50-pytorch</t>
+  </si>
+  <si>
+    <t>PyTorch</t>
+  </si>
+  <si>
+    <t>76.15%</t>
+  </si>
+  <si>
+    <t>92.87%</t>
+  </si>
+  <si>
+    <t>squeezenet1.1</t>
+  </si>
+  <si>
+    <t>58.38%</t>
+  </si>
+  <si>
+    <t>81.01%</t>
   </si>
   <si>
     <t>efficientnet-b0</t>
   </si>
   <si>
-    <t>27.78%</t>
-  </si>
-  <si>
-    <t>44.40%</t>
-  </si>
-  <si>
-    <t>googlenet-v1</t>
-  </si>
-  <si>
-    <t>Caffe</t>
-  </si>
-  <si>
-    <t>68.92%</t>
-  </si>
-  <si>
-    <t>89.14%</t>
-  </si>
-  <si>
-    <t>googlenet-v4-tf</t>
-  </si>
-  <si>
-    <t>80.21%</t>
-  </si>
-  <si>
-    <t>95.19%</t>
-  </si>
-  <si>
-    <t>resnet50-pytorch</t>
-  </si>
-  <si>
-    <t>PyTorch</t>
-  </si>
-  <si>
-    <t>76.15%</t>
-  </si>
-  <si>
-    <t>92.87%</t>
-  </si>
-  <si>
-    <t>squeezenet1.1</t>
-  </si>
-  <si>
-    <t>44.58%</t>
-  </si>
-  <si>
-    <t>70.03%</t>
+    <t>75.69%</t>
+  </si>
+  <si>
+    <t>92.76%</t>
   </si>
 </sst>
 </file>
@@ -679,7 +676,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
@@ -696,7 +693,7 @@
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,11 +712,8 @@
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -728,11 +722,8 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -741,11 +732,8 @@
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -754,226 +742,187 @@
       <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1111,40 +1060,6 @@
       <formula>LEN(TRIM(F5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="27">
-      <formula>LEN(TRIM(G1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="32">
-      <formula>LEN(TRIM(G16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="25">
-      <formula>LEN(TRIM(G2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="26">
-      <formula>LEN(TRIM(G2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="28">
-      <formula>LEN(TRIM(G4))&gt;0</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="8" priority="31">
-      <formula>LEN(TRIM(G4))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G15">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="29">
-      <formula>LEN(TRIM(G5))&gt;0</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="30">
-      <formula>LEN(TRIM(G5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>